<commit_message>
Development: - Borda score as method for the best solution added
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Studium\ISS\firefly\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5BD419-DCFA-402F-BCFF-319B529095D9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6D87D6-F155-4A1A-B450-A2BF7C4D3C5F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{7A5777CE-EC2E-432C-83CF-BE8066FBB872}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A5777CE-EC2E-432C-83CF-BE8066FBB872}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -257,28 +257,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1353,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041F0CE5-28EA-4617-BCB5-42EBFC5B924D}">
   <dimension ref="A2:G199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179:C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,156 +1389,102 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
         <f>COUNTIF($C$4:$C$198,0)</f>
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
         <f>COUNTIF($C$4:$C$198,1)</f>
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>27</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
         <f>COUNTIF($C$4:$C$198,2)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
       <c r="F7">
         <v>3</v>
       </c>
       <c r="G7">
         <f>COUNTIF($C$4:$C$198,3)</f>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>59</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="G8">
         <f>COUNTIF($C$4:$C$198,4)</f>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="G9">
         <f>COUNTIF($C$4:$C$198,5)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="F10">
         <v>6</v>
       </c>
       <c r="G10">
         <f>COUNTIF($C$4:$C$198,6)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
       <c r="F11">
         <v>7</v>
       </c>
       <c r="G11">
         <f>COUNTIF($C$4:$C$198,7)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12">
-        <v>23</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
       <c r="F12">
         <v>8</v>
       </c>
@@ -1551,12 +1497,6 @@
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13">
-        <v>16</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="F13">
         <v>9</v>
       </c>
@@ -1569,12 +1509,6 @@
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14">
-        <v>14</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
       <c r="F14">
         <v>10</v>
       </c>
@@ -1587,56 +1521,26 @@
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16">
-        <v>59</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17">
-        <v>23</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18">
-        <v>32</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19">
-        <v>13</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
       <c r="F19" t="s">
         <v>15</v>
       </c>
@@ -1645,61 +1549,37 @@
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20">
-        <v>25</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="F20">
+      <c r="F20" t="e">
         <f>SUM(G4,G5)/SUM(G4:G14)</f>
-        <v>0.66049382716049387</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21">
-        <v>39</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22">
-        <v>20</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23">
-        <v>64</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="e">
         <f>AVERAGE(B4:B23)</f>
-        <v>25.75</v>
-      </c>
-      <c r="C24">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C24" t="e">
         <f>AVERAGE(C4:C23)</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,233 +1605,113 @@
       <c r="A29">
         <v>1</v>
       </c>
-      <c r="B29">
-        <v>32</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
-      <c r="B30">
-        <v>62</v>
-      </c>
-      <c r="C30">
-        <v>7</v>
-      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
-      <c r="B31">
-        <v>84</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
-      <c r="B32">
-        <v>58</v>
-      </c>
-      <c r="C32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5</v>
       </c>
-      <c r="B33">
-        <v>43</v>
-      </c>
-      <c r="C33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6</v>
       </c>
-      <c r="B34">
-        <v>36</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7</v>
       </c>
-      <c r="B35">
-        <v>46</v>
-      </c>
-      <c r="C35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8</v>
       </c>
-      <c r="B36">
-        <v>46</v>
-      </c>
-      <c r="C36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9</v>
       </c>
-      <c r="B37">
-        <v>40</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10</v>
       </c>
-      <c r="B38">
-        <v>55</v>
-      </c>
-      <c r="C38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>11</v>
       </c>
-      <c r="B39">
-        <v>74</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12</v>
       </c>
-      <c r="B40">
-        <v>23</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>13</v>
       </c>
-      <c r="B41">
-        <v>61</v>
-      </c>
-      <c r="C41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>14</v>
       </c>
-      <c r="B42">
-        <v>20</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>15</v>
       </c>
-      <c r="B43">
-        <v>60</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>16</v>
       </c>
-      <c r="B44">
-        <v>33</v>
-      </c>
-      <c r="C44">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>17</v>
       </c>
-      <c r="B45">
-        <v>50</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>18</v>
       </c>
-      <c r="B46">
-        <v>37</v>
-      </c>
-      <c r="C46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>19</v>
       </c>
-      <c r="B47">
-        <v>46</v>
-      </c>
-      <c r="C47">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20</v>
-      </c>
-      <c r="B48">
-        <v>38</v>
-      </c>
-      <c r="C48">
-        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
-      <c r="B49">
+      <c r="B49" t="e">
         <f>AVERAGE(B29:B48)</f>
-        <v>47.2</v>
-      </c>
-      <c r="C49">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C49" t="e">
         <f>AVERAGE(C29:C48)</f>
-        <v>3.35</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1977,233 +1737,113 @@
       <c r="A54">
         <v>1</v>
       </c>
-      <c r="B54">
-        <v>39</v>
-      </c>
-      <c r="C54">
-        <v>3</v>
-      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
-      <c r="B55">
-        <v>58</v>
-      </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
-      <c r="B56">
-        <v>50</v>
-      </c>
-      <c r="C56">
-        <v>4</v>
-      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4</v>
       </c>
-      <c r="B57">
-        <v>31</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5</v>
       </c>
-      <c r="B58">
-        <v>44</v>
-      </c>
-      <c r="C58">
-        <v>5</v>
-      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6</v>
       </c>
-      <c r="B59">
-        <v>65</v>
-      </c>
-      <c r="C59">
-        <v>3</v>
-      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>7</v>
       </c>
-      <c r="B60">
-        <v>77</v>
-      </c>
-      <c r="C60">
-        <v>4</v>
-      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>8</v>
       </c>
-      <c r="B61">
-        <v>38</v>
-      </c>
-      <c r="C61">
-        <v>3</v>
-      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9</v>
       </c>
-      <c r="B62">
-        <v>58</v>
-      </c>
-      <c r="C62">
-        <v>3</v>
-      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>10</v>
       </c>
-      <c r="B63">
-        <v>35</v>
-      </c>
-      <c r="C63">
-        <v>3</v>
-      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>11</v>
       </c>
-      <c r="B64">
-        <v>32</v>
-      </c>
-      <c r="C64">
-        <v>5</v>
-      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>12</v>
       </c>
-      <c r="B65">
-        <v>33</v>
-      </c>
-      <c r="C65">
-        <v>3</v>
-      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>13</v>
       </c>
-      <c r="B66">
-        <v>50</v>
-      </c>
-      <c r="C66">
-        <v>3</v>
-      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>14</v>
       </c>
-      <c r="B67">
-        <v>56</v>
-      </c>
-      <c r="C67">
-        <v>2</v>
-      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>15</v>
       </c>
-      <c r="B68">
-        <v>20</v>
-      </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>16</v>
       </c>
-      <c r="B69">
-        <v>81</v>
-      </c>
-      <c r="C69">
-        <v>5</v>
-      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>17</v>
       </c>
-      <c r="B70">
-        <v>37</v>
-      </c>
-      <c r="C70">
-        <v>4</v>
-      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>18</v>
       </c>
-      <c r="B71">
-        <v>52</v>
-      </c>
-      <c r="C71">
-        <v>3</v>
-      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>19</v>
       </c>
-      <c r="B72">
-        <v>62</v>
-      </c>
-      <c r="C72">
-        <v>2</v>
-      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>20</v>
       </c>
-      <c r="B73">
-        <v>80</v>
-      </c>
-      <c r="C73">
-        <v>3</v>
-      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>13</v>
       </c>
-      <c r="B74">
+      <c r="B74" t="e">
         <f>AVERAGE(B54:B73)</f>
-        <v>49.9</v>
-      </c>
-      <c r="C74">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C74" t="e">
         <f>AVERAGE(C54:C73)</f>
-        <v>3.15</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2229,233 +1869,113 @@
       <c r="A79">
         <v>1</v>
       </c>
-      <c r="B79">
-        <v>98</v>
-      </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2</v>
       </c>
-      <c r="B80">
-        <v>64</v>
-      </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3</v>
       </c>
-      <c r="B81">
-        <v>309</v>
-      </c>
-      <c r="C81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4</v>
       </c>
-      <c r="B82">
-        <v>50</v>
-      </c>
-      <c r="C82">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5</v>
       </c>
-      <c r="B83">
-        <v>74</v>
-      </c>
-      <c r="C83">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>6</v>
       </c>
-      <c r="B84">
-        <v>35</v>
-      </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>7</v>
       </c>
-      <c r="B85">
-        <v>411</v>
-      </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>8</v>
       </c>
-      <c r="B86">
-        <v>38</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>9</v>
       </c>
-      <c r="B87">
-        <v>101</v>
-      </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>10</v>
       </c>
-      <c r="B88">
-        <v>23</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>11</v>
       </c>
-      <c r="B89">
-        <v>65</v>
-      </c>
-      <c r="C89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>12</v>
       </c>
-      <c r="B90">
-        <v>42</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>13</v>
       </c>
-      <c r="B91">
-        <v>57</v>
-      </c>
-      <c r="C91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>14</v>
       </c>
-      <c r="B92">
-        <v>68</v>
-      </c>
-      <c r="C92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>15</v>
       </c>
-      <c r="B93">
-        <v>429</v>
-      </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>16</v>
       </c>
-      <c r="B94">
-        <v>625</v>
-      </c>
-      <c r="C94">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>17</v>
       </c>
-      <c r="B95">
-        <v>737</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>18</v>
-      </c>
-      <c r="B96">
-        <v>95</v>
-      </c>
-      <c r="C96">
-        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>19</v>
       </c>
-      <c r="B97">
-        <v>442</v>
-      </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>20</v>
       </c>
-      <c r="B98">
-        <v>158</v>
-      </c>
-      <c r="C98">
-        <v>2</v>
-      </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>13</v>
       </c>
-      <c r="B99">
+      <c r="B99" t="e">
         <f>AVERAGE(B79:B98)</f>
-        <v>196.05</v>
-      </c>
-      <c r="C99">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C99" t="e">
         <f>AVERAGE(C79:C98)</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2481,233 +2001,113 @@
       <c r="A104">
         <v>1</v>
       </c>
-      <c r="B104">
-        <v>38</v>
-      </c>
-      <c r="C104">
-        <v>2</v>
-      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2</v>
       </c>
-      <c r="B105">
-        <v>36</v>
-      </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>3</v>
       </c>
-      <c r="B106">
-        <v>59</v>
-      </c>
-      <c r="C106">
-        <v>1</v>
-      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>4</v>
       </c>
-      <c r="B107">
-        <v>61</v>
-      </c>
-      <c r="C107">
-        <v>0</v>
-      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>5</v>
       </c>
-      <c r="B108">
-        <v>38</v>
-      </c>
-      <c r="C108">
-        <v>0</v>
-      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>6</v>
       </c>
-      <c r="B109">
-        <v>40</v>
-      </c>
-      <c r="C109">
-        <v>1</v>
-      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>7</v>
       </c>
-      <c r="B110">
-        <v>57</v>
-      </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>8</v>
       </c>
-      <c r="B111">
-        <v>55</v>
-      </c>
-      <c r="C111">
-        <v>0</v>
-      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>9</v>
       </c>
-      <c r="B112">
-        <v>32</v>
-      </c>
-      <c r="C112">
-        <v>0</v>
-      </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>10</v>
       </c>
-      <c r="B113">
-        <v>44</v>
-      </c>
-      <c r="C113">
-        <v>0</v>
-      </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>11</v>
       </c>
-      <c r="B114">
-        <v>88</v>
-      </c>
-      <c r="C114">
-        <v>1</v>
-      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>12</v>
       </c>
-      <c r="B115">
-        <v>36</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>13</v>
       </c>
-      <c r="B116">
-        <v>45</v>
-      </c>
-      <c r="C116">
-        <v>1</v>
-      </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>14</v>
       </c>
-      <c r="B117">
-        <v>55</v>
-      </c>
-      <c r="C117">
-        <v>1</v>
-      </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>15</v>
       </c>
-      <c r="B118">
-        <v>37</v>
-      </c>
-      <c r="C118">
-        <v>0</v>
-      </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>16</v>
       </c>
-      <c r="B119">
-        <v>93</v>
-      </c>
-      <c r="C119">
-        <v>1</v>
-      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>17</v>
       </c>
-      <c r="B120">
-        <v>49</v>
-      </c>
-      <c r="C120">
-        <v>0</v>
-      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>18</v>
       </c>
-      <c r="B121">
-        <v>90</v>
-      </c>
-      <c r="C121">
-        <v>0</v>
-      </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>19</v>
       </c>
-      <c r="B122">
-        <v>40</v>
-      </c>
-      <c r="C122">
-        <v>0</v>
-      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>20</v>
       </c>
-      <c r="B123">
-        <v>86</v>
-      </c>
-      <c r="C123">
-        <v>0</v>
-      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>13</v>
       </c>
-      <c r="B124">
+      <c r="B124" t="e">
         <f>AVERAGE(B104:B123)</f>
-        <v>53.95</v>
-      </c>
-      <c r="C124">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C124" t="e">
         <f>AVERAGE(C104:C123)</f>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -2729,237 +2129,117 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1</v>
       </c>
-      <c r="B129">
-        <v>90</v>
-      </c>
-      <c r="C129">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2</v>
       </c>
-      <c r="B130">
-        <v>72</v>
-      </c>
-      <c r="C130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>3</v>
       </c>
-      <c r="B131">
-        <v>93</v>
-      </c>
-      <c r="C131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>4</v>
       </c>
-      <c r="B132">
-        <v>115</v>
-      </c>
-      <c r="C132">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>5</v>
       </c>
-      <c r="B133">
-        <v>141</v>
-      </c>
-      <c r="C133">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>6</v>
       </c>
-      <c r="B134">
-        <v>151</v>
-      </c>
-      <c r="C134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>7</v>
       </c>
-      <c r="B135">
-        <v>94</v>
-      </c>
-      <c r="C135">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>8</v>
       </c>
-      <c r="B136">
-        <v>27</v>
-      </c>
-      <c r="C136">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>9</v>
       </c>
-      <c r="B137">
-        <v>168</v>
-      </c>
-      <c r="C137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>10</v>
       </c>
-      <c r="B138">
-        <v>62</v>
-      </c>
-      <c r="C138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>11</v>
       </c>
-      <c r="B139">
-        <v>111</v>
-      </c>
-      <c r="C139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>12</v>
       </c>
-      <c r="B140">
-        <v>87</v>
-      </c>
-      <c r="C140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>13</v>
       </c>
-      <c r="B141">
-        <v>74</v>
-      </c>
-      <c r="C141">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>14</v>
       </c>
-      <c r="B142">
-        <v>125</v>
-      </c>
-      <c r="C142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>15</v>
       </c>
-      <c r="B143">
-        <v>87</v>
-      </c>
-      <c r="C143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>16</v>
-      </c>
-      <c r="B144">
-        <v>86</v>
-      </c>
-      <c r="C144">
-        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>17</v>
       </c>
-      <c r="B145">
-        <v>68</v>
-      </c>
-      <c r="C145">
-        <v>4</v>
-      </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>18</v>
       </c>
-      <c r="B146">
-        <v>96</v>
-      </c>
-      <c r="C146">
-        <v>1</v>
-      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>19</v>
       </c>
-      <c r="B147">
-        <v>64</v>
-      </c>
-      <c r="C147">
-        <v>1</v>
-      </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>20</v>
       </c>
-      <c r="B148">
-        <v>116</v>
-      </c>
-      <c r="C148">
-        <v>0</v>
-      </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>13</v>
       </c>
-      <c r="B149">
+      <c r="B149" t="e">
         <f>AVERAGE(B129:B148)</f>
-        <v>96.35</v>
-      </c>
-      <c r="C149">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C149" t="e">
         <f>AVERAGE(C129:C148)</f>
-        <v>1.4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2985,233 +2265,113 @@
       <c r="A154">
         <v>1</v>
       </c>
-      <c r="B154">
-        <v>10</v>
-      </c>
-      <c r="C154">
-        <v>0</v>
-      </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2</v>
       </c>
-      <c r="B155">
-        <v>9</v>
-      </c>
-      <c r="C155">
-        <v>0</v>
-      </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>3</v>
       </c>
-      <c r="B156">
-        <v>9</v>
-      </c>
-      <c r="C156">
-        <v>0</v>
-      </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>4</v>
       </c>
-      <c r="B157">
-        <v>19</v>
-      </c>
-      <c r="C157">
-        <v>0</v>
-      </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>5</v>
       </c>
-      <c r="B158">
-        <v>9</v>
-      </c>
-      <c r="C158">
-        <v>0</v>
-      </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>6</v>
       </c>
-      <c r="B159">
-        <v>10</v>
-      </c>
-      <c r="C159">
-        <v>0</v>
-      </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>7</v>
       </c>
-      <c r="B160">
-        <v>12</v>
-      </c>
-      <c r="C160">
-        <v>0</v>
-      </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>8</v>
       </c>
-      <c r="B161">
-        <v>12</v>
-      </c>
-      <c r="C161">
-        <v>3</v>
-      </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>9</v>
       </c>
-      <c r="B162">
-        <v>9</v>
-      </c>
-      <c r="C162">
-        <v>0</v>
-      </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>10</v>
       </c>
-      <c r="B163">
-        <v>11</v>
-      </c>
-      <c r="C163">
-        <v>4</v>
-      </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>11</v>
       </c>
-      <c r="B164">
-        <v>15</v>
-      </c>
-      <c r="C164">
-        <v>0</v>
-      </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>12</v>
       </c>
-      <c r="B165">
-        <v>12</v>
-      </c>
-      <c r="C165">
-        <v>0</v>
-      </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>13</v>
       </c>
-      <c r="B166">
-        <v>15</v>
-      </c>
-      <c r="C166">
-        <v>0</v>
-      </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>14</v>
       </c>
-      <c r="B167">
-        <v>9</v>
-      </c>
-      <c r="C167">
-        <v>0</v>
-      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>15</v>
       </c>
-      <c r="B168">
-        <v>11</v>
-      </c>
-      <c r="C168">
-        <v>0</v>
-      </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>16</v>
       </c>
-      <c r="B169">
-        <v>8</v>
-      </c>
-      <c r="C169">
-        <v>0</v>
-      </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>17</v>
       </c>
-      <c r="B170">
-        <v>8</v>
-      </c>
-      <c r="C170">
-        <v>0</v>
-      </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>18</v>
       </c>
-      <c r="B171">
-        <v>10</v>
-      </c>
-      <c r="C171">
-        <v>2</v>
-      </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>19</v>
       </c>
-      <c r="B172">
-        <v>12</v>
-      </c>
-      <c r="C172">
-        <v>3</v>
-      </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>20</v>
       </c>
-      <c r="B173">
-        <v>9</v>
-      </c>
-      <c r="C173">
-        <v>2</v>
-      </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>13</v>
       </c>
-      <c r="B174">
+      <c r="B174" t="e">
         <f>AVERAGE(B154:B173)</f>
-        <v>10.95</v>
-      </c>
-      <c r="C174">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C174" t="e">
         <f>AVERAGE(C154:C173)</f>
-        <v>0.7</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -3237,233 +2397,113 @@
       <c r="A179">
         <v>1</v>
       </c>
-      <c r="B179">
-        <v>8</v>
-      </c>
-      <c r="C179">
-        <v>0</v>
-      </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2</v>
       </c>
-      <c r="B180">
-        <v>12</v>
-      </c>
-      <c r="C180">
-        <v>0</v>
-      </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>3</v>
       </c>
-      <c r="B181">
-        <v>7</v>
-      </c>
-      <c r="C181">
-        <v>0</v>
-      </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>4</v>
       </c>
-      <c r="B182">
-        <v>8</v>
-      </c>
-      <c r="C182">
-        <v>0</v>
-      </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>5</v>
       </c>
-      <c r="B183">
-        <v>8</v>
-      </c>
-      <c r="C183">
-        <v>0</v>
-      </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>6</v>
       </c>
-      <c r="B184">
-        <v>8</v>
-      </c>
-      <c r="C184">
-        <v>0</v>
-      </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>7</v>
       </c>
-      <c r="B185">
-        <v>8</v>
-      </c>
-      <c r="C185">
-        <v>0</v>
-      </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>8</v>
       </c>
-      <c r="B186">
-        <v>9</v>
-      </c>
-      <c r="C186">
-        <v>0</v>
-      </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>9</v>
       </c>
-      <c r="B187">
-        <v>8</v>
-      </c>
-      <c r="C187">
-        <v>0</v>
-      </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>10</v>
       </c>
-      <c r="B188">
-        <v>9</v>
-      </c>
-      <c r="C188">
-        <v>0</v>
-      </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>11</v>
       </c>
-      <c r="B189">
-        <v>7</v>
-      </c>
-      <c r="C189">
-        <v>0</v>
-      </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>12</v>
       </c>
-      <c r="B190">
-        <v>8</v>
-      </c>
-      <c r="C190">
-        <v>0</v>
-      </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>13</v>
       </c>
-      <c r="B191">
-        <v>8</v>
-      </c>
-      <c r="C191">
-        <v>0</v>
-      </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>14</v>
       </c>
-      <c r="B192">
-        <v>8</v>
-      </c>
-      <c r="C192">
-        <v>0</v>
-      </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>15</v>
       </c>
-      <c r="B193">
-        <v>9</v>
-      </c>
-      <c r="C193">
-        <v>0</v>
-      </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>16</v>
       </c>
-      <c r="B194">
-        <v>8</v>
-      </c>
-      <c r="C194">
-        <v>0</v>
-      </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>17</v>
       </c>
-      <c r="B195">
-        <v>9</v>
-      </c>
-      <c r="C195">
-        <v>0</v>
-      </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>18</v>
       </c>
-      <c r="B196">
-        <v>8</v>
-      </c>
-      <c r="C196">
-        <v>0</v>
-      </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>19</v>
       </c>
-      <c r="B197">
-        <v>8</v>
-      </c>
-      <c r="C197">
-        <v>0</v>
-      </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>20</v>
       </c>
-      <c r="B198">
-        <v>8</v>
-      </c>
-      <c r="C198">
-        <v>0</v>
-      </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>13</v>
       </c>
-      <c r="B199">
+      <c r="B199" t="e">
         <f>AVERAGE(B179:B198)</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="C199">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C199" t="e">
         <f>AVERAGE(C179:C198)</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New data + remove problem 09
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Studium\ISS\firefly\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6D87D6-F155-4A1A-B450-A2BF7C4D3C5F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC7CF84-4979-4D2B-8E46-3054A446D305}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A5777CE-EC2E-432C-83CF-BE8066FBB872}"/>
   </bookViews>
@@ -257,13 +257,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -272,7 +272,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1354,7 +1354,7 @@
   <dimension ref="A2:G199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179:C198"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,47 +1389,71 @@
       <c r="A4">
         <v>1</v>
       </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <f>COUNTIF($C$4:$C$198,0)</f>
-        <v>0</v>
+        <f>COUNTIF($C$4:$C$224,0)</f>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <f>COUNTIF($C$4:$C$198,1)</f>
-        <v>0</v>
+        <f>COUNTIF($C$4:$C$224,1)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
-        <f>COUNTIF($C$4:$C$198,2)</f>
-        <v>0</v>
+        <f>COUNTIF($C$4:$C$224,2)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="F7">
         <v>3</v>
       </c>
       <c r="G7">
-        <f>COUNTIF($C$4:$C$198,3)</f>
+        <f>COUNTIF($C$4:$C$224,3)</f>
         <v>0</v>
       </c>
     </row>
@@ -1437,11 +1461,17 @@
       <c r="A8">
         <v>5</v>
       </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="G8">
-        <f>COUNTIF($C$4:$C$198,4)</f>
+        <f>COUNTIF($C$4:$C$224,4)</f>
         <v>0</v>
       </c>
     </row>
@@ -1449,23 +1479,35 @@
       <c r="A9">
         <v>6</v>
       </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="G9">
-        <f>COUNTIF($C$4:$C$198,5)</f>
-        <v>0</v>
+        <f>COUNTIF($C$4:$C$224,5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
       <c r="F10">
         <v>6</v>
       </c>
       <c r="G10">
-        <f>COUNTIF($C$4:$C$198,6)</f>
+        <f>COUNTIF($C$4:$C$224,6)</f>
         <v>0</v>
       </c>
     </row>
@@ -1473,11 +1515,17 @@
       <c r="A11">
         <v>8</v>
       </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
       <c r="F11">
         <v>7</v>
       </c>
       <c r="G11">
-        <f>COUNTIF($C$4:$C$198,7)</f>
+        <f>COUNTIF($C$4:$C$224,7)</f>
         <v>0</v>
       </c>
     </row>
@@ -1485,11 +1533,17 @@
       <c r="A12">
         <v>9</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
       <c r="F12">
         <v>8</v>
       </c>
       <c r="G12">
-        <f>COUNTIF($C$4:$C$198,8)</f>
+        <f>COUNTIF($C$4:$C$224,8)</f>
         <v>0</v>
       </c>
     </row>
@@ -1497,11 +1551,17 @@
       <c r="A13">
         <v>10</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
       <c r="F13">
         <v>9</v>
       </c>
       <c r="G13">
-        <f>COUNTIF($C$4:$C$198,9)</f>
+        <f>COUNTIF($C$4:$C$224,9)</f>
         <v>0</v>
       </c>
     </row>
@@ -1509,11 +1569,17 @@
       <c r="A14">
         <v>11</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="F14">
         <v>10</v>
       </c>
       <c r="G14">
-        <f>COUNTIF($C$4:$C$198,10)</f>
+        <f>COUNTIF($C$4:$C$224,10)</f>
         <v>0</v>
       </c>
     </row>
@@ -1521,26 +1587,56 @@
       <c r="A15">
         <v>12</v>
       </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
       <c r="F19" t="s">
         <v>15</v>
       </c>
@@ -1549,37 +1645,57 @@
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="F20" t="e">
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="F20">
         <f>SUM(G4,G5)/SUM(G4:G14)</f>
-        <v>#DIV/0!</v>
+        <v>0.98124999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24" t="e">
+      <c r="B24">
         <f>AVERAGE(B4:B23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C24" t="e">
-        <f>AVERAGE(C4:C23)</f>
-        <v>#DIV/0!</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1605,113 +1721,229 @@
       <c r="A29">
         <v>1</v>
       </c>
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
+      <c r="B30">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
+      <c r="B31">
+        <v>13</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>21</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>21</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>29</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>24</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>24</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>16</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>18</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>26</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>19</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>19</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>13</v>
       </c>
-      <c r="B49" t="e">
+      <c r="B49">
         <f>AVERAGE(B29:B48)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C49" t="e">
-        <f>AVERAGE(C29:C48)</f>
-        <v>#DIV/0!</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1737,113 +1969,229 @@
       <c r="A54">
         <v>1</v>
       </c>
+      <c r="B54">
+        <v>18</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
+      <c r="B55">
+        <v>18</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
+      <c r="B56">
+        <v>27</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4</v>
       </c>
+      <c r="B57">
+        <v>28</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5</v>
       </c>
+      <c r="B58">
+        <v>42</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6</v>
       </c>
+      <c r="B59">
+        <v>16</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>7</v>
       </c>
+      <c r="B60">
+        <v>29</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>8</v>
       </c>
+      <c r="B61">
+        <v>22</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9</v>
       </c>
+      <c r="B62">
+        <v>38</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>10</v>
       </c>
+      <c r="B63">
+        <v>28</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>11</v>
       </c>
+      <c r="B64">
+        <v>32</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>12</v>
       </c>
+      <c r="B65">
+        <v>27</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>13</v>
       </c>
+      <c r="B66">
+        <v>24</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>14</v>
       </c>
+      <c r="B67">
+        <v>24</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>15</v>
       </c>
+      <c r="B68">
+        <v>19</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>16</v>
       </c>
+      <c r="B69">
+        <v>34</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>17</v>
       </c>
+      <c r="B70">
+        <v>26</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>18</v>
       </c>
+      <c r="B71">
+        <v>19</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>19</v>
       </c>
+      <c r="B72">
+        <v>16</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>20</v>
       </c>
+      <c r="B73">
+        <v>17</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>13</v>
       </c>
-      <c r="B74" t="e">
+      <c r="B74">
         <f>AVERAGE(B54:B73)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C74" t="e">
-        <f>AVERAGE(C54:C73)</f>
-        <v>#DIV/0!</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1869,113 +2217,229 @@
       <c r="A79">
         <v>1</v>
       </c>
+      <c r="B79">
+        <v>20</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>27</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>6</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>5</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>300</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>6</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>23</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>8</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>9</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>26</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>10</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>11</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>21</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>12</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>14</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>13</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>300</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>14</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>11</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>15</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>6</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>16</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>300</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>17</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>11</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>18</v>
+      </c>
+      <c r="B96">
+        <v>12</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>19</v>
       </c>
+      <c r="B97">
+        <v>15</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>20</v>
       </c>
+      <c r="B98">
+        <v>16</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>13</v>
       </c>
-      <c r="B99" t="e">
+      <c r="B99">
         <f>AVERAGE(B79:B98)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C99" t="e">
-        <f>AVERAGE(C79:C98)</f>
-        <v>#DIV/0!</v>
+        <v>56.4</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2001,113 +2465,229 @@
       <c r="A104">
         <v>1</v>
       </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2</v>
       </c>
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>3</v>
       </c>
+      <c r="B106">
+        <v>4</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>4</v>
       </c>
+      <c r="B107">
+        <v>2</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>5</v>
       </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>6</v>
       </c>
+      <c r="B109">
+        <v>3</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>7</v>
       </c>
+      <c r="B110">
+        <v>3</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>8</v>
       </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>9</v>
       </c>
+      <c r="B112">
+        <v>3</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>10</v>
       </c>
+      <c r="B113">
+        <v>2</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>11</v>
       </c>
+      <c r="B114">
+        <v>9</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>12</v>
       </c>
+      <c r="B115">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>13</v>
       </c>
+      <c r="B116">
+        <v>5</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>14</v>
       </c>
+      <c r="B117">
+        <v>3</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>15</v>
       </c>
+      <c r="B118">
+        <v>4</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>16</v>
       </c>
+      <c r="B119">
+        <v>3</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>17</v>
       </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>18</v>
       </c>
+      <c r="B121">
+        <v>3</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>19</v>
       </c>
+      <c r="B122">
+        <v>2</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>20</v>
       </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>13</v>
       </c>
-      <c r="B124" t="e">
+      <c r="B124">
         <f>AVERAGE(B104:B123)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C124" t="e">
-        <f>AVERAGE(C104:C123)</f>
-        <v>#DIV/0!</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -2129,117 +2709,233 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>4</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>8</v>
+      </c>
+      <c r="C130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>3</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>8</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>4</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>3</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>5</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>4</v>
+      </c>
+      <c r="C133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>6</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>2</v>
+      </c>
+      <c r="C134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>7</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>4</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>8</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>6</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>9</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>4</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>10</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>2</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>11</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>2</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>12</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>4</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>13</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>5</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>14</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>12</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>15</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>4</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>16</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>17</v>
       </c>
+      <c r="B145">
+        <v>6</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>18</v>
       </c>
+      <c r="B146">
+        <v>4</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>19</v>
       </c>
+      <c r="B147">
+        <v>4</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>20</v>
       </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>13</v>
       </c>
-      <c r="B149" t="e">
+      <c r="B149">
         <f>AVERAGE(B129:B148)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C149" t="e">
-        <f>AVERAGE(C129:C148)</f>
-        <v>#DIV/0!</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -2265,113 +2961,229 @@
       <c r="A154">
         <v>1</v>
       </c>
+      <c r="B154">
+        <v>11</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2</v>
       </c>
+      <c r="B155">
+        <v>20</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>3</v>
       </c>
+      <c r="B156">
+        <v>22</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>4</v>
       </c>
+      <c r="B157">
+        <v>16</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>5</v>
       </c>
+      <c r="B158">
+        <v>18</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>6</v>
       </c>
+      <c r="B159">
+        <v>7</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>7</v>
       </c>
+      <c r="B160">
+        <v>9</v>
+      </c>
+      <c r="C160">
+        <v>0</v>
+      </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>8</v>
       </c>
+      <c r="B161">
+        <v>12</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>9</v>
       </c>
+      <c r="B162">
+        <v>7</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>10</v>
       </c>
+      <c r="B163">
+        <v>11</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>11</v>
       </c>
+      <c r="B164">
+        <v>12</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>12</v>
       </c>
+      <c r="B165">
+        <v>14</v>
+      </c>
+      <c r="C165">
+        <v>0</v>
+      </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>13</v>
       </c>
+      <c r="B166">
+        <v>12</v>
+      </c>
+      <c r="C166">
+        <v>2</v>
+      </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>14</v>
       </c>
+      <c r="B167">
+        <v>19</v>
+      </c>
+      <c r="C167">
+        <v>0</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>15</v>
       </c>
+      <c r="B168">
+        <v>10</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>16</v>
       </c>
+      <c r="B169">
+        <v>9</v>
+      </c>
+      <c r="C169">
+        <v>0</v>
+      </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>17</v>
       </c>
+      <c r="B170">
+        <v>11</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>18</v>
       </c>
+      <c r="B171">
+        <v>7</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>19</v>
       </c>
+      <c r="B172">
+        <v>9</v>
+      </c>
+      <c r="C172">
+        <v>0</v>
+      </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>20</v>
       </c>
+      <c r="B173">
+        <v>9</v>
+      </c>
+      <c r="C173">
+        <v>0</v>
+      </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>13</v>
       </c>
-      <c r="B174" t="e">
+      <c r="B174">
         <f>AVERAGE(B154:B173)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C174" t="e">
-        <f>AVERAGE(C154:C173)</f>
-        <v>#DIV/0!</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2397,113 +3209,229 @@
       <c r="A179">
         <v>1</v>
       </c>
+      <c r="B179">
+        <v>8</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2</v>
       </c>
+      <c r="B180">
+        <v>11</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>3</v>
       </c>
+      <c r="B181">
+        <v>8</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>4</v>
       </c>
+      <c r="B182">
+        <v>7</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>5</v>
       </c>
+      <c r="B183">
+        <v>14</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>6</v>
       </c>
+      <c r="B184">
+        <v>12</v>
+      </c>
+      <c r="C184">
+        <v>0</v>
+      </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>7</v>
       </c>
+      <c r="B185">
+        <v>5</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>8</v>
       </c>
+      <c r="B186">
+        <v>8</v>
+      </c>
+      <c r="C186">
+        <v>0</v>
+      </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>9</v>
       </c>
+      <c r="B187">
+        <v>5</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>10</v>
       </c>
+      <c r="B188">
+        <v>13</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>11</v>
       </c>
+      <c r="B189">
+        <v>4</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>12</v>
       </c>
+      <c r="B190">
+        <v>5</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>13</v>
       </c>
+      <c r="B191">
+        <v>12</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
+      </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>14</v>
       </c>
+      <c r="B192">
+        <v>16</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>15</v>
       </c>
+      <c r="B193">
+        <v>14</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>16</v>
       </c>
+      <c r="B194">
+        <v>15</v>
+      </c>
+      <c r="C194">
+        <v>0</v>
+      </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>17</v>
       </c>
+      <c r="B195">
+        <v>7</v>
+      </c>
+      <c r="C195">
+        <v>0</v>
+      </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>18</v>
       </c>
+      <c r="B196">
+        <v>14</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>19</v>
       </c>
+      <c r="B197">
+        <v>9</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>20</v>
       </c>
+      <c r="B198">
+        <v>16</v>
+      </c>
+      <c r="C198">
+        <v>0</v>
+      </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>13</v>
       </c>
-      <c r="B199" t="e">
+      <c r="B199">
         <f>AVERAGE(B179:B198)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C199" t="e">
-        <f>AVERAGE(C179:C198)</f>
-        <v>#DIV/0!</v>
+        <v>10.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>